<commit_message>
modified excel with reports + found new code error
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\Desktop\AN 3-SEM 2\VVSS\labs\proiect-lab\Echipa-jamilei\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A214A60B-F212-4E79-A06F-77CBE39D21D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E33BFF-CFF4-412D-82CE-A66847033462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="2010" windowWidth="16200" windowHeight="9398" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="428" yWindow="1132" windowWidth="16200" windowHeight="9398" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -168,19 +168,56 @@
   </si>
   <si>
     <t>paragraf nou adaugat dupa primul paragraf</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>service package -&gt; PaymentAlertGUI</t>
+  </si>
+  <si>
+    <t>In clasa PaymentAlertGUI este prezentata logica de GUI pentru afisarea unei ferestre de confirmare si printarea In consola a anumitor evenimente. Din punct de vedere logic aceasta clasa ar trebui sa fie situata in pachetul de gui si nu in cel de service</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>KithcenGUIController/51</t>
+  </si>
+  <si>
+    <t>Nu a fost tratat cazul in care nu era selectat niciun Order si astfel aparea o eroare</t>
+  </si>
+  <si>
+    <t>KithcenGUIController/63</t>
+  </si>
+  <si>
+    <t>OrdersGUIController/112,139</t>
+  </si>
+  <si>
+    <t>Se putea apasa pe butonul de "Place order" fara a exista vreun item selectat. L-am facut disabled pana cand se adauga un prim item la un order.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -359,80 +396,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +814,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J4" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -822,7 +860,7 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="37" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="21" t="s">
@@ -843,7 +881,7 @@
       <c r="I4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="37" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1079,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1124,8 +1162,12 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="7" t="s">
@@ -1138,8 +1180,12 @@
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="7" t="s">
@@ -1184,13 +1230,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
@@ -1364,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1410,8 +1462,12 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="16" t="s">
@@ -1424,8 +1480,12 @@
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="16" t="s">
@@ -1470,31 +1530,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3">

</xml_diff>

<commit_message>
Changed the KitchenGUI name. Fixed some more errors in the MainGUIController and actualized the Architectural Design Phase file
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\Desktop\AN 3-SEM 2\VVSS\labs\proiect-lab\Echipa-jamilei\Docs\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Materii\03_PizzaShop\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E33BFF-CFF4-412D-82CE-A66847033462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485615EA-27CC-4C9C-BD77-7B0898E86FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="428" yWindow="1132" windowWidth="16200" windowHeight="9398" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -173,9 +173,6 @@
     <t>A02</t>
   </si>
   <si>
-    <t>service package -&gt; PaymentAlertGUI</t>
-  </si>
-  <si>
     <t>In clasa PaymentAlertGUI este prezentata logica de GUI pentru afisarea unei ferestre de confirmare si printarea In consola a anumitor evenimente. Din punct de vedere logic aceasta clasa ar trebui sa fie situata in pachetul de gui si nu in cel de service</t>
   </si>
   <si>
@@ -198,6 +195,27 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Nu se valideaza corect ca resursa  a putut fi incarcata. Se afiseaza o eroare la consola si se continua cu o valoare nula, care va face sa esueze mai departe functia</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>service/PaymentAlertGUI</t>
+  </si>
+  <si>
+    <t>gui/KitchenGUI:16</t>
+  </si>
+  <si>
+    <t>controller/MainGUIController:59</t>
+  </si>
+  <si>
+    <t>Functia tableHandlers se apeleaza in functia setService. Nu se urmeaza principiul singurei responsabilitati, cum aceasta functie ar trebuie doar sa seteze valoarea pentru service. Un loc mai potrivit pentru apelul acestei functii este in initialize</t>
   </si>
 </sst>
 </file>
@@ -428,6 +446,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -470,7 +489,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,36 +836,36 @@
       <selection activeCell="J4" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.3984375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.86328125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.3984375" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.86328125" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -856,65 +874,65 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -928,7 +946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -942,7 +960,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -957,7 +975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -972,7 +990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -981,7 +999,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -990,7 +1008,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -999,7 +1017,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1008,7 +1026,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1017,7 +1035,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1026,7 +1044,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1035,7 +1053,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1044,7 +1062,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1053,7 +1071,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1062,7 +1080,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1071,7 +1089,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1080,7 +1098,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1089,7 +1107,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1117,39 +1135,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.3984375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.86328125" style="6"/>
-    <col min="9" max="9" width="22.06640625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.86328125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1158,65 +1176,65 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1238,31 +1256,43 @@
         <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1271,7 +1301,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1280,7 +1310,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1289,7 +1319,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1298,7 +1328,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1307,7 +1337,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1316,7 +1346,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1325,7 +1355,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1334,7 +1364,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1343,7 +1373,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1352,7 +1382,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1361,7 +1391,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1370,7 +1400,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1379,7 +1409,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1388,7 +1418,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1416,40 +1446,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.3984375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.86328125" style="6"/>
-    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.86328125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1458,65 +1488,65 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="23" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1530,51 +1560,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1583,7 +1613,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1592,7 +1622,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1601,7 +1631,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1610,7 +1640,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1619,7 +1649,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1628,7 +1658,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1637,7 +1667,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1646,7 +1676,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1655,7 +1685,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1664,7 +1694,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1673,7 +1703,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1682,7 +1712,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1691,7 +1721,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1700,7 +1730,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1709,7 +1739,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1718,7 +1748,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1727,7 +1757,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1736,7 +1766,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1768,37 +1798,37 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.9296875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.86328125" style="6"/>
-    <col min="9" max="9" width="26.73046875" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.86328125" style="6"/>
+    <col min="5" max="5" width="23.88671875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="25" t="s">
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1807,47 +1837,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1864,7 +1894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1873,7 +1903,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1883,7 +1913,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1893,7 +1923,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1903,7 +1933,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1913,7 +1943,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1923,7 +1953,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1933,7 +1963,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1943,7 +1973,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1953,7 +1983,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1963,7 +1993,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1973,7 +2003,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1983,7 +2013,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1993,7 +2023,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2003,7 +2033,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2013,7 +2043,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2023,7 +2053,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2033,7 +2063,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2043,7 +2073,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2053,7 +2083,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2063,7 +2093,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2073,12 +2103,12 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="C32" s="35" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added modified class diagram
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Materii\03_PizzaShop\Docs\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\Desktop\AN 3-SEM 2\VVSS\labs\proiect-lab\Echipa-jamilei\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485615EA-27CC-4C9C-BD77-7B0898E86FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C89AA4-EB24-43FD-A77D-1E63974A0ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="4628" windowWidth="16200" windowHeight="9397" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>Functia tableHandlers se apeleaza in functia setService. Nu se urmeaza principiul singurei responsabilitati, cum aceasta functie ar trebuie doar sa seteze valoarea pentru service. Un loc mai potrivit pentru apelul acestei functii este in initialize</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>KithcenGUIController/15</t>
+  </si>
+  <si>
+    <t>Nu era specificat tipul elementelor din kitchenOrdersList. Am adaugat generic type String la acea lista</t>
   </si>
 </sst>
 </file>
@@ -836,19 +845,19 @@
       <selection activeCell="J4" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.86328125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.46484375" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="6"/>
+    <col min="10" max="10" width="14.46484375" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.86328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -859,7 +868,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
@@ -874,7 +883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
@@ -885,7 +894,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -903,7 +912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -917,7 +926,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -925,14 +934,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -946,7 +955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -960,7 +969,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -975,7 +984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -990,7 +999,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -999,7 +1008,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1008,7 +1017,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1017,7 +1026,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1026,7 +1035,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1035,7 +1044,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1044,7 +1053,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1053,7 +1062,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1062,7 +1071,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1071,7 +1080,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1080,7 +1089,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1089,7 +1098,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1098,7 +1107,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1107,7 +1116,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1135,22 +1144,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.86328125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.46484375" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="6"/>
+    <col min="9" max="9" width="22.1328125" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1161,7 +1170,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1219,7 +1228,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1227,14 +1236,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1262,7 +1271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1277,7 +1286,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1292,7 +1301,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1301,7 +1310,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1310,7 +1319,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1319,7 +1328,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1328,7 +1337,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1337,7 +1346,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1346,7 +1355,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1355,7 +1364,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1364,7 +1373,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1373,7 +1382,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1382,7 +1391,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1391,7 +1400,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1400,7 +1409,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1409,7 +1418,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1418,7 +1427,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1446,23 +1455,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.86328125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="41.46484375" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.86328125" style="6"/>
+    <col min="9" max="9" width="26.796875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1473,7 +1482,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1526,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +1540,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1539,14 +1548,14 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1589,7 +1598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1604,16 +1613,22 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1622,7 +1637,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1631,7 +1646,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1640,7 +1655,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1649,7 +1664,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1658,7 +1673,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1667,7 +1682,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1676,7 +1691,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1685,7 +1700,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1694,7 +1709,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1703,7 +1718,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1712,7 +1727,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1721,7 +1736,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1730,7 +1745,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1739,7 +1754,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1748,7 +1763,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1757,7 +1772,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1766,7 +1781,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1798,20 +1813,20 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="8.86328125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="23.86328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.53125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" style="6"/>
+    <col min="9" max="9" width="26.796875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.86328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1822,7 +1837,7 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B2" s="26" t="s">
         <v>30</v>
       </c>
@@ -1837,14 +1852,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
@@ -1856,7 +1871,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1868,7 +1883,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1877,7 +1892,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1894,7 +1909,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1903,7 +1918,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1913,7 +1928,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1923,7 +1938,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1933,7 +1948,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1943,7 +1958,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1953,7 +1968,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1963,7 +1978,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1973,7 +1988,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1983,7 +1998,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1993,7 +2008,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2003,7 +2018,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2013,7 +2028,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2023,7 +2038,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2033,7 +2048,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2043,7 +2058,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2053,7 +2068,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2063,7 +2078,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2073,7 +2088,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2083,7 +2098,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2093,7 +2108,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2103,7 +2118,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C32" s="36" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
added last sonarLint issue in excel
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\Desktop\AN 3-SEM 2\VVSS\labs\proiect-lab\Echipa-jamilei\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066B066B-3583-4228-B05D-6F793631C8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C8B887-8BA0-4B9E-9B1E-B4266FBCB0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1628" yWindow="1830" windowWidth="16199" windowHeight="9398" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -272,6 +272,19 @@
   </si>
   <si>
     <t>if ((l==null) ||(l.isEmpty())) return total;</t>
+  </si>
+  <si>
+    <t>PaymentAlertGUI/52</t>
+  </si>
+  <si>
+    <t>Se face get pe o variabila optional fara sa se verifice inainte daca este prezenta o valoare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional&lt;ButtonType&gt; result = paymentAlert.showAndWait();
+        if (result.get() == cardPayment) </t>
+  </si>
+  <si>
+    <t>Este ok deoarece clasa Alert e implementata astfel incat tot timpul returneaza o valoare</t>
   </si>
 </sst>
 </file>
@@ -1856,8 +1869,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2025,15 +2038,23 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B15" s="3">

</xml_diff>